<commit_message>
Update de casos de prueba
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce3\Documents\GitHub\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E91B1145-21B7-416E-B7E4-063879288EE3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456C080C-5B88-412A-B0FC-EFC2B7A3BADA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="18510" windowHeight="15600" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="131">
   <si>
     <t>TC_001</t>
   </si>
@@ -348,18 +348,11 @@
     <t>Paso</t>
   </si>
   <si>
-    <t>Pedir un producto específico(foto mayor a 5 MB)</t>
-  </si>
-  <si>
     <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
 2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
 3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 7 Mbytes
 4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:ddd, Ciudad: Cordoba
 5. El solicitante selecciona la opcion "Siguiente"</t>
-  </si>
-  <si>
-    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
-5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y el sistema muestra mensaje de error "Tamaño de foto mayor a 5 MB" y "Numero de direccion debe ser numerico"</t>
   </si>
   <si>
     <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
@@ -426,6 +419,99 @@
   </si>
   <si>
     <t>18,19,20,21</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante no ingresa una descripción del Producto
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante no ingresa la direccion del comercio en forma textual y no ingresa un punto del mapa desde Google Maps
+5. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y el sistema muestra mensaje de error "No ingreso una descripcion del producto" y "No ingreso una direccion valida ni selecciono una ubicacion en el mapa"</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(foto con formato distinto de JPG)</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato PNG y con un tamaño de 5 Mbytes
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:567, Ciudad: Cordoba
+5. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>El sistema permite el ingreso de fotos de formato distinto de JPG</t>
+  </si>
+  <si>
+    <t>1. Ingresar al sistema para Pedir "lo que sea".
+2. Ingresar una descripción del Producto "Auriculares Bluethoot Philips"
+3. Adjuntar una foto de los auriculares en formato PNG y con un tamaño de 5 MBytes
+4. Ingresar la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:567, Ciudad: Cordoba
+5. Releccionar la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(sin descripcion ni direccion de comercio)</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(sin direccion de entrega)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante selecciona la direccion del comercio de desde el mapa de Google Maps
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante no ingresa la direccion de entrega
+7. El solicitante selecciona la opcion "Siguiente"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y muestra mensaje de error "El formato de la foto adjuntada no es JPG" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio se selecciono desde Google Maps y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra un mensaje de error "No ingreso una direccion de entrega".
+</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(foto mayor a 5 MB y letras en el campo Nro. De la direccion de comercio)</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(con letras en el campo Nro. De la direccion de entrega)</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y muestra mensaje de error "Tamaño de foto mayor a 5 MB" y "Numero de direccion debe ser numerico"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio se selecciono desde Google Maps y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra mensaje de error "Numero de direccion de entrega debe ser numerico"</t>
+  </si>
+  <si>
+    <t>El sistema permite el ingreso de letras en el campo Nro de la direccion de entrega</t>
+  </si>
+  <si>
+    <t>1.Ingresar al sistema para Pedir "lo que sea".
+2. Ingresar una descripción del Producto "Auriculares Bluethoot Philips"
+3. Adjuntar una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. Seleccionar la direccion del comercio de desde el mapa de Google Maps
+5. Seleccionar la opcion "Siguiente"
+6. Ingresar la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: ddd, y seleccionar la ciudad Ciudad: Capital
+7. Seleccionar la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante selecciona la direccion del comercio de desde el mapa de Google Maps
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: ddd, y selecciona la ciudad Ciudad: Capital
+7. El solicitante selecciona la opcion "Siguiente"</t>
   </si>
 </sst>
 </file>
@@ -1794,9 +1880,9 @@
   </sheetPr>
   <dimension ref="A1:AS69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2017,7 +2103,7 @@
         <v>72</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>74</v>
@@ -2104,10 +2190,10 @@
         <v>96</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H7" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>98</v>
@@ -2154,10 +2240,10 @@
         <v>97</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>98</v>
@@ -2201,13 +2287,13 @@
         <v>92</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H9" s="46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>98</v>
@@ -2245,22 +2331,22 @@
         <v>5.14</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="E10" s="47" t="s">
         <v>87</v>
       </c>
       <c r="F10" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="H10" s="56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J10" s="58"/>
       <c r="K10" s="59">
@@ -2286,20 +2372,34 @@
       <c r="AR10" s="54"/>
       <c r="AS10" s="54"/>
     </row>
-    <row r="11" spans="1:45" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" s="11" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="47" t="s">
+        <v>88</v>
+      </c>
       <c r="C11" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="57"/>
+      <c r="G11" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" s="57" t="s">
+        <v>98</v>
+      </c>
       <c r="J11" s="58"/>
       <c r="K11" s="59"/>
       <c r="L11" s="60"/>
@@ -2320,23 +2420,41 @@
       <c r="AR11" s="54"/>
       <c r="AS11" s="54"/>
     </row>
-    <row r="12" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" s="11" customFormat="1" ht="132" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="C12" s="22">
         <v>6</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="57"/>
+      <c r="D12" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="57" t="s">
+        <v>105</v>
+      </c>
       <c r="J12" s="58"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="60"/>
+      <c r="K12" s="59">
+        <v>2</v>
+      </c>
+      <c r="L12" s="60">
+        <v>43755</v>
+      </c>
       <c r="M12" s="34"/>
       <c r="N12" s="57"/>
       <c r="O12" s="58"/>
@@ -2354,20 +2472,34 @@
       <c r="AR12" s="54"/>
       <c r="AS12" s="54"/>
     </row>
-    <row r="13" spans="1:45" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" s="11" customFormat="1" ht="204" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="C13" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="57"/>
+        <v>112</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="57" t="s">
+        <v>98</v>
+      </c>
       <c r="J13" s="58"/>
       <c r="K13" s="59"/>
       <c r="L13" s="60"/>
@@ -2388,23 +2520,41 @@
       <c r="AR13" s="54"/>
       <c r="AS13" s="54"/>
     </row>
-    <row r="14" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.2">
       <c r="A14" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="C14" s="22">
         <v>22</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="57"/>
+      <c r="D14" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="57" t="s">
+        <v>105</v>
+      </c>
       <c r="J14" s="58"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="60"/>
+      <c r="K14" s="59">
+        <v>3</v>
+      </c>
+      <c r="L14" s="60">
+        <v>43755</v>
+      </c>
       <c r="M14" s="34"/>
       <c r="N14" s="57"/>
       <c r="O14" s="58"/>
@@ -4397,8 +4547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4467,44 +4617,72 @@
         <v>43755</v>
       </c>
       <c r="D4" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>111</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>86</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="39">
+        <v>43755</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>3</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="B6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="39">
+        <v>43755</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
@@ -4820,15 +4998,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
se agregan casos de 9,10,11 y 12
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce3\Documents\GitHub\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Desktop\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E91B1145-21B7-416E-B7E4-063879288EE3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7E5B72-221E-4B23-A2DE-ECD39CAAD5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
   <si>
     <t>TC_001</t>
   </si>
@@ -426,6 +426,102 @@
   </si>
   <si>
     <t>18,19,20,21</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(monto negativo para pagar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85, y selecciona la ciudad Ciudad: Capital
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago contado e ingresa una cantidad de $-800
+9. El solicitante selecciona la opcion "Siguiente"
+</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que el monto ingresado sea un monto positivo, y es invalido.
+El sistema muestra un mensaje de error "Monto invalido".</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(No selecciona forma de pago)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85, y selecciona la ciudad Ciudad: Capital
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante NO selecciona forma de pago. 
+9. El solicitante selecciona la opcion "Siguiente"
+</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que se seleccione una  forma de pago y no es asi 
+El sistema muestra un mensaje de error "Debe seleccionar una forma de pago".</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9.  El sistema valida que se seleccione una  forma de pago y no es asi 
+El sistema muestra un mensaje de error "Debe seleccionar una forma de pago".</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(Con tarjeta ingresando mal el numero de tarjeta)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 1111 1111 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC 123
+9. El solicitante selecciona la opcion "Siguiente"
+</t>
+  </si>
+  <si>
+    <t>Ciudad de Capital debe estar cargada en el sistema.</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de creditosea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "La tarjeta tiene que ser visa"</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(ingresando datos distintos del titular)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC 123
+9. El solicitante selecciona la opcion "Siguiente"
+</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de creditosea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "los datos ingresados, no coinciden con los del titular de la tarjeta"</t>
   </si>
 </sst>
 </file>
@@ -932,24 +1028,6 @@
     <xf numFmtId="14" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -965,12 +1043,6 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1001,6 +1073,30 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1014,7 +1110,399 @@
     <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="103">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1794,12 +2282,12 @@
   </sheetPr>
   <dimension ref="A1:AS69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
@@ -1826,113 +2314,113 @@
     <col min="23" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="50" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:45" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-    </row>
-    <row r="2" spans="1:45" s="50" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="51"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+    </row>
+    <row r="2" spans="1:45" s="44" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="45"/>
+      <c r="AN2" s="45"/>
+      <c r="AO2" s="45"/>
+      <c r="AP2" s="45"/>
+      <c r="AQ2" s="45"/>
+      <c r="AR2" s="45"/>
+      <c r="AS2" s="45"/>
     </row>
     <row r="3" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="38"/>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="59"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
@@ -1959,36 +2447,36 @@
       <c r="AD3" s="4"/>
     </row>
     <row r="4" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="40" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40" t="s">
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40" t="s">
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-    </row>
-    <row r="5" spans="1:45" ht="36" x14ac:dyDescent="0.2">
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+    </row>
+    <row r="5" spans="1:45" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>65</v>
       </c>
@@ -2100,13 +2588,13 @@
       <c r="E7" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="40" t="s">
         <v>102</v>
       </c>
       <c r="I7" s="15" t="s">
@@ -2114,10 +2602,10 @@
       </c>
       <c r="J7" s="29"/>
       <c r="K7" s="32"/>
-      <c r="L7" s="49">
+      <c r="L7" s="43">
         <v>43754</v>
       </c>
-      <c r="M7" s="48"/>
+      <c r="M7" s="42"/>
       <c r="N7" s="28"/>
       <c r="O7" s="29"/>
       <c r="P7" s="16"/>
@@ -2134,7 +2622,7 @@
       <c r="AR7" s="7"/>
       <c r="AS7" s="7"/>
     </row>
-    <row r="8" spans="1:45" ht="300" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" ht="288" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>40</v>
       </c>
@@ -2150,13 +2638,13 @@
       <c r="E8" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="40" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="15" t="s">
@@ -2164,7 +2652,7 @@
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="29"/>
-      <c r="L8" s="49">
+      <c r="L8" s="43">
         <v>43755</v>
       </c>
       <c r="M8" s="34"/>
@@ -2184,7 +2672,7 @@
       <c r="AR8" s="7"/>
       <c r="AS8" s="7"/>
     </row>
-    <row r="9" spans="1:45" ht="276" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" ht="264" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>41</v>
       </c>
@@ -2200,13 +2688,13 @@
       <c r="E9" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="40" t="s">
         <v>104</v>
       </c>
       <c r="I9" s="15" t="s">
@@ -2214,7 +2702,7 @@
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="29"/>
-      <c r="L9" s="49">
+      <c r="L9" s="43">
         <v>43754</v>
       </c>
       <c r="M9" s="34"/>
@@ -2235,10 +2723,10 @@
       <c r="AS9" s="7"/>
     </row>
     <row r="10" spans="1:45" s="11" customFormat="1" ht="132" x14ac:dyDescent="0.2">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="41" t="s">
         <v>88</v>
       </c>
       <c r="C10" s="22">
@@ -2247,81 +2735,80 @@
       <c r="D10" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I10" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="58"/>
-      <c r="K10" s="59">
+      <c r="J10" s="50"/>
+      <c r="K10" s="51">
         <v>1</v>
       </c>
-      <c r="L10" s="60">
+      <c r="L10" s="52">
         <v>43755</v>
       </c>
       <c r="M10" s="34"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="61"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="53"/>
       <c r="R10" s="34"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="58"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="61"/>
-      <c r="AN10" s="54"/>
-      <c r="AO10" s="54"/>
-      <c r="AP10" s="54"/>
-      <c r="AQ10" s="54"/>
-      <c r="AR10" s="54"/>
-      <c r="AS10" s="54"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="53"/>
+      <c r="AN10" s="46"/>
+      <c r="AO10" s="46"/>
+      <c r="AP10" s="46"/>
+      <c r="AQ10" s="46"/>
+      <c r="AR10" s="46"/>
+      <c r="AS10" s="46"/>
     </row>
     <row r="11" spans="1:45" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="56"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="26"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="60"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="52"/>
       <c r="M11" s="34"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="61"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="53"/>
       <c r="R11" s="34"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="58"/>
-      <c r="U11" s="59"/>
-      <c r="V11" s="61"/>
-      <c r="AN11" s="54"/>
-      <c r="AO11" s="54"/>
-      <c r="AP11" s="54"/>
-      <c r="AQ11" s="54"/>
-      <c r="AR11" s="54"/>
-      <c r="AS11" s="54"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="51"/>
+      <c r="V11" s="53"/>
+      <c r="AN11" s="46"/>
+      <c r="AO11" s="46"/>
+      <c r="AP11" s="46"/>
+      <c r="AQ11" s="46"/>
+      <c r="AR11" s="46"/>
+      <c r="AS11" s="46"/>
     </row>
     <row r="12" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="47" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="22"/>
@@ -2333,29 +2820,29 @@
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="60"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="52"/>
       <c r="M12" s="34"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="61"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="53"/>
       <c r="R12" s="34"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="59"/>
-      <c r="V12" s="61"/>
-      <c r="AN12" s="54"/>
-      <c r="AO12" s="54"/>
-      <c r="AP12" s="54"/>
-      <c r="AQ12" s="54"/>
-      <c r="AR12" s="54"/>
-      <c r="AS12" s="54"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="53"/>
+      <c r="AN12" s="46"/>
+      <c r="AO12" s="46"/>
+      <c r="AP12" s="46"/>
+      <c r="AQ12" s="46"/>
+      <c r="AR12" s="46"/>
+      <c r="AS12" s="46"/>
     </row>
     <row r="13" spans="1:45" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="47" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="22"/>
@@ -2367,29 +2854,29 @@
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="60"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="52"/>
       <c r="M13" s="34"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="61"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="53"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="61"/>
-      <c r="AN13" s="54"/>
-      <c r="AO13" s="54"/>
-      <c r="AP13" s="54"/>
-      <c r="AQ13" s="54"/>
-      <c r="AR13" s="54"/>
-      <c r="AS13" s="54"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="53"/>
+      <c r="AN13" s="46"/>
+      <c r="AO13" s="46"/>
+      <c r="AP13" s="46"/>
+      <c r="AQ13" s="46"/>
+      <c r="AR13" s="46"/>
+      <c r="AS13" s="46"/>
     </row>
     <row r="14" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="47" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="22"/>
@@ -2401,165 +2888,227 @@
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="60"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="52"/>
       <c r="M14" s="34"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="61"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="53"/>
       <c r="R14" s="34"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="59"/>
-      <c r="V14" s="61"/>
-      <c r="AN14" s="54"/>
-      <c r="AO14" s="54"/>
-      <c r="AP14" s="54"/>
-      <c r="AQ14" s="54"/>
-      <c r="AR14" s="54"/>
-      <c r="AS14" s="54"/>
-    </row>
-    <row r="15" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
+      <c r="S14" s="49"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="53"/>
+      <c r="AN14" s="46"/>
+      <c r="AO14" s="46"/>
+      <c r="AP14" s="46"/>
+      <c r="AQ14" s="46"/>
+      <c r="AR14" s="46"/>
+      <c r="AS14" s="46"/>
+    </row>
+    <row r="15" spans="1:45" s="11" customFormat="1" ht="240" x14ac:dyDescent="0.2">
+      <c r="A15" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="C15" s="22">
         <v>25</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="60"/>
+      <c r="D15" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" s="26"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52">
+        <v>43755</v>
+      </c>
       <c r="M15" s="34"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="61"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="53"/>
       <c r="R15" s="34"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="61"/>
-      <c r="AN15" s="54"/>
-      <c r="AO15" s="54"/>
-      <c r="AP15" s="54"/>
-      <c r="AQ15" s="54"/>
-      <c r="AR15" s="54"/>
-      <c r="AS15" s="54"/>
-    </row>
-    <row r="16" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
+      <c r="S15" s="49"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="53"/>
+      <c r="AN15" s="46"/>
+      <c r="AO15" s="46"/>
+      <c r="AP15" s="46"/>
+      <c r="AQ15" s="46"/>
+      <c r="AR15" s="46"/>
+      <c r="AS15" s="46"/>
+    </row>
+    <row r="16" spans="1:45" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="22"/>
       <c r="C16" s="22">
         <v>26</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="60"/>
+      <c r="D16" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="52">
+        <v>43755</v>
+      </c>
       <c r="M16" s="34"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="61"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="53"/>
       <c r="R16" s="34"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="58"/>
-      <c r="U16" s="59"/>
-      <c r="V16" s="61"/>
-      <c r="AN16" s="54"/>
-      <c r="AO16" s="54"/>
-      <c r="AP16" s="54"/>
-      <c r="AQ16" s="54"/>
-      <c r="AR16" s="54"/>
-      <c r="AS16" s="54"/>
-    </row>
-    <row r="17" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
+      <c r="S16" s="49"/>
+      <c r="T16" s="50"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="53"/>
+      <c r="AN16" s="46"/>
+      <c r="AO16" s="46"/>
+      <c r="AP16" s="46"/>
+      <c r="AQ16" s="46"/>
+      <c r="AR16" s="46"/>
+      <c r="AS16" s="46"/>
+    </row>
+    <row r="17" spans="1:45" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.2">
+      <c r="A17" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22">
+      <c r="B17" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="21">
         <v>27</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="60"/>
+      <c r="D17" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="52">
+        <v>43755</v>
+      </c>
       <c r="M17" s="34"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="61"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="53"/>
       <c r="R17" s="34"/>
-      <c r="S17" s="57"/>
-      <c r="T17" s="58"/>
-      <c r="U17" s="59"/>
-      <c r="V17" s="61"/>
-      <c r="AN17" s="54"/>
-      <c r="AO17" s="54"/>
-      <c r="AP17" s="54"/>
-      <c r="AQ17" s="54"/>
-      <c r="AR17" s="54"/>
-      <c r="AS17" s="54"/>
-    </row>
-    <row r="18" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="55" t="s">
+      <c r="S17" s="49"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="53"/>
+      <c r="AN17" s="46"/>
+      <c r="AO17" s="46"/>
+      <c r="AP17" s="46"/>
+      <c r="AQ17" s="46"/>
+      <c r="AR17" s="46"/>
+      <c r="AS17" s="46"/>
+    </row>
+    <row r="18" spans="1:45" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="C18" s="22">
         <v>28</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="60"/>
+      <c r="D18" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="50"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="52">
+        <v>43755</v>
+      </c>
       <c r="M18" s="34"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="61"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="53"/>
       <c r="R18" s="34"/>
-      <c r="S18" s="57"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="61"/>
-      <c r="AN18" s="54"/>
-      <c r="AO18" s="54"/>
-      <c r="AP18" s="54"/>
-      <c r="AQ18" s="54"/>
-      <c r="AR18" s="54"/>
-      <c r="AS18" s="54"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="53"/>
+      <c r="AN18" s="46"/>
+      <c r="AO18" s="46"/>
+      <c r="AP18" s="46"/>
+      <c r="AQ18" s="46"/>
+      <c r="AR18" s="46"/>
+      <c r="AS18" s="46"/>
     </row>
     <row r="19" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="47" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="22"/>
@@ -2571,29 +3120,29 @@
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="60"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="52"/>
       <c r="M19" s="34"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="61"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="53"/>
       <c r="R19" s="34"/>
-      <c r="S19" s="57"/>
-      <c r="T19" s="58"/>
-      <c r="U19" s="59"/>
-      <c r="V19" s="61"/>
-      <c r="AN19" s="54"/>
-      <c r="AO19" s="54"/>
-      <c r="AP19" s="54"/>
-      <c r="AQ19" s="54"/>
-      <c r="AR19" s="54"/>
-      <c r="AS19" s="54"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="53"/>
+      <c r="AN19" s="46"/>
+      <c r="AO19" s="46"/>
+      <c r="AP19" s="46"/>
+      <c r="AQ19" s="46"/>
+      <c r="AR19" s="46"/>
+      <c r="AS19" s="46"/>
     </row>
     <row r="20" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="47" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="22"/>
@@ -2605,29 +3154,29 @@
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="60"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="52"/>
       <c r="M20" s="34"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="61"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="53"/>
       <c r="R20" s="34"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="59"/>
-      <c r="V20" s="61"/>
-      <c r="AN20" s="54"/>
-      <c r="AO20" s="54"/>
-      <c r="AP20" s="54"/>
-      <c r="AQ20" s="54"/>
-      <c r="AR20" s="54"/>
-      <c r="AS20" s="54"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="53"/>
+      <c r="AN20" s="46"/>
+      <c r="AO20" s="46"/>
+      <c r="AP20" s="46"/>
+      <c r="AQ20" s="46"/>
+      <c r="AR20" s="46"/>
+      <c r="AS20" s="46"/>
     </row>
     <row r="21" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="47" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="22"/>
@@ -2639,29 +3188,29 @@
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="60"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="52"/>
       <c r="M21" s="34"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="61"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="53"/>
       <c r="R21" s="34"/>
-      <c r="S21" s="57"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="59"/>
-      <c r="V21" s="61"/>
-      <c r="AN21" s="54"/>
-      <c r="AO21" s="54"/>
-      <c r="AP21" s="54"/>
-      <c r="AQ21" s="54"/>
-      <c r="AR21" s="54"/>
-      <c r="AS21" s="54"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="53"/>
+      <c r="AN21" s="46"/>
+      <c r="AO21" s="46"/>
+      <c r="AP21" s="46"/>
+      <c r="AQ21" s="46"/>
+      <c r="AR21" s="46"/>
+      <c r="AS21" s="46"/>
     </row>
     <row r="22" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="47" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="22"/>
@@ -2673,29 +3222,29 @@
       <c r="F22" s="26"/>
       <c r="G22" s="26"/>
       <c r="H22" s="26"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="60"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="52"/>
       <c r="M22" s="34"/>
-      <c r="N22" s="57"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="61"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="53"/>
       <c r="R22" s="34"/>
-      <c r="S22" s="57"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="59"/>
-      <c r="V22" s="61"/>
-      <c r="AN22" s="54"/>
-      <c r="AO22" s="54"/>
-      <c r="AP22" s="54"/>
-      <c r="AQ22" s="54"/>
-      <c r="AR22" s="54"/>
-      <c r="AS22" s="54"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="50"/>
+      <c r="U22" s="51"/>
+      <c r="V22" s="53"/>
+      <c r="AN22" s="46"/>
+      <c r="AO22" s="46"/>
+      <c r="AP22" s="46"/>
+      <c r="AQ22" s="46"/>
+      <c r="AR22" s="46"/>
+      <c r="AS22" s="46"/>
     </row>
     <row r="23" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="22"/>
@@ -2705,29 +3254,29 @@
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="60"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="52"/>
       <c r="M23" s="34"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="58"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="61"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="53"/>
       <c r="R23" s="34"/>
-      <c r="S23" s="57"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="59"/>
-      <c r="V23" s="61"/>
-      <c r="AN23" s="54"/>
-      <c r="AO23" s="54"/>
-      <c r="AP23" s="54"/>
-      <c r="AQ23" s="54"/>
-      <c r="AR23" s="54"/>
-      <c r="AS23" s="54"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="51"/>
+      <c r="V23" s="53"/>
+      <c r="AN23" s="46"/>
+      <c r="AO23" s="46"/>
+      <c r="AP23" s="46"/>
+      <c r="AQ23" s="46"/>
+      <c r="AR23" s="46"/>
+      <c r="AS23" s="46"/>
     </row>
     <row r="24" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="47" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="22"/>
@@ -2737,29 +3286,29 @@
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="60"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="52"/>
       <c r="M24" s="34"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="61"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="53"/>
       <c r="R24" s="34"/>
-      <c r="S24" s="57"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="59"/>
-      <c r="V24" s="61"/>
-      <c r="AN24" s="54"/>
-      <c r="AO24" s="54"/>
-      <c r="AP24" s="54"/>
-      <c r="AQ24" s="54"/>
-      <c r="AR24" s="54"/>
-      <c r="AS24" s="54"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="51"/>
+      <c r="V24" s="53"/>
+      <c r="AN24" s="46"/>
+      <c r="AO24" s="46"/>
+      <c r="AP24" s="46"/>
+      <c r="AQ24" s="46"/>
+      <c r="AR24" s="46"/>
+      <c r="AS24" s="46"/>
     </row>
     <row r="25" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="47" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="22"/>
@@ -2769,29 +3318,29 @@
       <c r="F25" s="26"/>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="60"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="52"/>
       <c r="M25" s="34"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="61"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="53"/>
       <c r="R25" s="34"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="59"/>
-      <c r="V25" s="61"/>
-      <c r="AN25" s="54"/>
-      <c r="AO25" s="54"/>
-      <c r="AP25" s="54"/>
-      <c r="AQ25" s="54"/>
-      <c r="AR25" s="54"/>
-      <c r="AS25" s="54"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="53"/>
+      <c r="AN25" s="46"/>
+      <c r="AO25" s="46"/>
+      <c r="AP25" s="46"/>
+      <c r="AQ25" s="46"/>
+      <c r="AR25" s="46"/>
+      <c r="AS25" s="46"/>
     </row>
     <row r="26" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="47" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="22"/>
@@ -2801,29 +3350,29 @@
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="60"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="52"/>
       <c r="M26" s="34"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="61"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="53"/>
       <c r="R26" s="34"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="61"/>
-      <c r="AN26" s="54"/>
-      <c r="AO26" s="54"/>
-      <c r="AP26" s="54"/>
-      <c r="AQ26" s="54"/>
-      <c r="AR26" s="54"/>
-      <c r="AS26" s="54"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="53"/>
+      <c r="AN26" s="46"/>
+      <c r="AO26" s="46"/>
+      <c r="AP26" s="46"/>
+      <c r="AQ26" s="46"/>
+      <c r="AR26" s="46"/>
+      <c r="AS26" s="46"/>
     </row>
     <row r="27" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="47" t="s">
         <v>59</v>
       </c>
       <c r="B27" s="22"/>
@@ -2833,125 +3382,125 @@
       <c r="F27" s="26"/>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="60"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="52"/>
       <c r="M27" s="34"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="61"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="53"/>
       <c r="R27" s="34"/>
-      <c r="S27" s="57"/>
-      <c r="T27" s="58"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="61"/>
-      <c r="AN27" s="54"/>
-      <c r="AO27" s="54"/>
-      <c r="AP27" s="54"/>
-      <c r="AQ27" s="54"/>
-      <c r="AR27" s="54"/>
-      <c r="AS27" s="54"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="53"/>
+      <c r="AN27" s="46"/>
+      <c r="AO27" s="46"/>
+      <c r="AP27" s="46"/>
+      <c r="AQ27" s="46"/>
+      <c r="AR27" s="46"/>
+      <c r="AS27" s="46"/>
     </row>
     <row r="28" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="55" t="s">
+      <c r="A28" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
       <c r="H28" s="26"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="60"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="52"/>
       <c r="M28" s="34"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="61"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="53"/>
       <c r="R28" s="34"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="61"/>
-      <c r="AN28" s="54"/>
-      <c r="AO28" s="54"/>
-      <c r="AP28" s="54"/>
-      <c r="AQ28" s="54"/>
-      <c r="AR28" s="54"/>
-      <c r="AS28" s="54"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="53"/>
+      <c r="AN28" s="46"/>
+      <c r="AO28" s="46"/>
+      <c r="AP28" s="46"/>
+      <c r="AQ28" s="46"/>
+      <c r="AR28" s="46"/>
+      <c r="AS28" s="46"/>
     </row>
     <row r="29" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
       <c r="H29" s="26"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="60"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="52"/>
       <c r="M29" s="34"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="58"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="61"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="53"/>
       <c r="R29" s="34"/>
-      <c r="S29" s="57"/>
-      <c r="T29" s="58"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="61"/>
-      <c r="AN29" s="54"/>
-      <c r="AO29" s="54"/>
-      <c r="AP29" s="54"/>
-      <c r="AQ29" s="54"/>
-      <c r="AR29" s="54"/>
-      <c r="AS29" s="54"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="51"/>
+      <c r="V29" s="53"/>
+      <c r="AN29" s="46"/>
+      <c r="AO29" s="46"/>
+      <c r="AP29" s="46"/>
+      <c r="AQ29" s="46"/>
+      <c r="AR29" s="46"/>
+      <c r="AS29" s="46"/>
     </row>
     <row r="30" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="47" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="26"/>
-      <c r="F30" s="46"/>
+      <c r="F30" s="40"/>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="60"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="52"/>
       <c r="M30" s="34"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="61"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="53"/>
       <c r="R30" s="34"/>
-      <c r="S30" s="57"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="59"/>
-      <c r="V30" s="61"/>
-      <c r="AN30" s="54"/>
-      <c r="AO30" s="54"/>
-      <c r="AP30" s="54"/>
-      <c r="AQ30" s="54"/>
-      <c r="AR30" s="54"/>
-      <c r="AS30" s="54"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="51"/>
+      <c r="V30" s="53"/>
+      <c r="AN30" s="46"/>
+      <c r="AO30" s="46"/>
+      <c r="AP30" s="46"/>
+      <c r="AQ30" s="46"/>
+      <c r="AR30" s="46"/>
+      <c r="AS30" s="46"/>
     </row>
     <row r="31" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="47" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="22"/>
@@ -2961,29 +3510,29 @@
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="60"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="52"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="61"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="53"/>
       <c r="R31" s="34"/>
-      <c r="S31" s="57"/>
-      <c r="T31" s="58"/>
-      <c r="U31" s="59"/>
-      <c r="V31" s="61"/>
-      <c r="AN31" s="54"/>
-      <c r="AO31" s="54"/>
-      <c r="AP31" s="54"/>
-      <c r="AQ31" s="54"/>
-      <c r="AR31" s="54"/>
-      <c r="AS31" s="54"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="53"/>
+      <c r="AN31" s="46"/>
+      <c r="AO31" s="46"/>
+      <c r="AP31" s="46"/>
+      <c r="AQ31" s="46"/>
+      <c r="AR31" s="46"/>
+      <c r="AS31" s="46"/>
     </row>
     <row r="32" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="47" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="22"/>
@@ -2993,29 +3542,29 @@
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="60"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="51"/>
+      <c r="L32" s="52"/>
       <c r="M32" s="34"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="61"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="51"/>
+      <c r="Q32" s="53"/>
       <c r="R32" s="34"/>
-      <c r="S32" s="57"/>
-      <c r="T32" s="58"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="61"/>
-      <c r="AN32" s="54"/>
-      <c r="AO32" s="54"/>
-      <c r="AP32" s="54"/>
-      <c r="AQ32" s="54"/>
-      <c r="AR32" s="54"/>
-      <c r="AS32" s="54"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="51"/>
+      <c r="V32" s="53"/>
+      <c r="AN32" s="46"/>
+      <c r="AO32" s="46"/>
+      <c r="AP32" s="46"/>
+      <c r="AQ32" s="46"/>
+      <c r="AR32" s="46"/>
+      <c r="AS32" s="46"/>
     </row>
     <row r="33" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="22"/>
@@ -3025,29 +3574,29 @@
       <c r="F33" s="26"/>
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="60"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="52"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="61"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="50"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="53"/>
       <c r="R33" s="34"/>
-      <c r="S33" s="57"/>
-      <c r="T33" s="58"/>
-      <c r="U33" s="59"/>
-      <c r="V33" s="61"/>
-      <c r="AN33" s="54"/>
-      <c r="AO33" s="54"/>
-      <c r="AP33" s="54"/>
-      <c r="AQ33" s="54"/>
-      <c r="AR33" s="54"/>
-      <c r="AS33" s="54"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="50"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="53"/>
+      <c r="AN33" s="46"/>
+      <c r="AO33" s="46"/>
+      <c r="AP33" s="46"/>
+      <c r="AQ33" s="46"/>
+      <c r="AR33" s="46"/>
+      <c r="AS33" s="46"/>
     </row>
     <row r="34" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="55" t="s">
+      <c r="A34" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="22"/>
@@ -3057,29 +3606,29 @@
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="60"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="52"/>
       <c r="M34" s="34"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="61"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="50"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="53"/>
       <c r="R34" s="34"/>
-      <c r="S34" s="57"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="59"/>
-      <c r="V34" s="61"/>
-      <c r="AN34" s="54"/>
-      <c r="AO34" s="54"/>
-      <c r="AP34" s="54"/>
-      <c r="AQ34" s="54"/>
-      <c r="AR34" s="54"/>
-      <c r="AS34" s="54"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="51"/>
+      <c r="V34" s="53"/>
+      <c r="AN34" s="46"/>
+      <c r="AO34" s="46"/>
+      <c r="AP34" s="46"/>
+      <c r="AQ34" s="46"/>
+      <c r="AR34" s="46"/>
+      <c r="AS34" s="46"/>
     </row>
     <row r="35" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="55" t="s">
+      <c r="A35" s="47" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="22"/>
@@ -3089,29 +3638,29 @@
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="59"/>
-      <c r="L35" s="60"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="52"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="59"/>
-      <c r="Q35" s="61"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="50"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="53"/>
       <c r="R35" s="34"/>
-      <c r="S35" s="57"/>
-      <c r="T35" s="58"/>
-      <c r="U35" s="59"/>
-      <c r="V35" s="61"/>
-      <c r="AN35" s="54"/>
-      <c r="AO35" s="54"/>
-      <c r="AP35" s="54"/>
-      <c r="AQ35" s="54"/>
-      <c r="AR35" s="54"/>
-      <c r="AS35" s="54"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="50"/>
+      <c r="U35" s="51"/>
+      <c r="V35" s="53"/>
+      <c r="AN35" s="46"/>
+      <c r="AO35" s="46"/>
+      <c r="AP35" s="46"/>
+      <c r="AQ35" s="46"/>
+      <c r="AR35" s="46"/>
+      <c r="AS35" s="46"/>
     </row>
     <row r="36" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="47" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="22"/>
@@ -3121,29 +3670,29 @@
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="60"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="52"/>
       <c r="M36" s="34"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="61"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="53"/>
       <c r="R36" s="34"/>
-      <c r="S36" s="57"/>
-      <c r="T36" s="58"/>
-      <c r="U36" s="59"/>
-      <c r="V36" s="61"/>
-      <c r="AN36" s="54"/>
-      <c r="AO36" s="54"/>
-      <c r="AP36" s="54"/>
-      <c r="AQ36" s="54"/>
-      <c r="AR36" s="54"/>
-      <c r="AS36" s="54"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="51"/>
+      <c r="V36" s="53"/>
+      <c r="AN36" s="46"/>
+      <c r="AO36" s="46"/>
+      <c r="AP36" s="46"/>
+      <c r="AQ36" s="46"/>
+      <c r="AR36" s="46"/>
+      <c r="AS36" s="46"/>
     </row>
     <row r="37" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="47" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="22"/>
@@ -3153,29 +3702,29 @@
       <c r="F37" s="26"/>
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="60"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="52"/>
       <c r="M37" s="34"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="61"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="53"/>
       <c r="R37" s="34"/>
-      <c r="S37" s="57"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="59"/>
-      <c r="V37" s="61"/>
-      <c r="AN37" s="54"/>
-      <c r="AO37" s="54"/>
-      <c r="AP37" s="54"/>
-      <c r="AQ37" s="54"/>
-      <c r="AR37" s="54"/>
-      <c r="AS37" s="54"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="50"/>
+      <c r="U37" s="51"/>
+      <c r="V37" s="53"/>
+      <c r="AN37" s="46"/>
+      <c r="AO37" s="46"/>
+      <c r="AP37" s="46"/>
+      <c r="AQ37" s="46"/>
+      <c r="AR37" s="46"/>
+      <c r="AS37" s="46"/>
     </row>
     <row r="38" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="47" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="22"/>
@@ -3185,29 +3734,29 @@
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="60"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="52"/>
       <c r="M38" s="34"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="58"/>
-      <c r="P38" s="59"/>
-      <c r="Q38" s="61"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="53"/>
       <c r="R38" s="34"/>
-      <c r="S38" s="57"/>
-      <c r="T38" s="58"/>
-      <c r="U38" s="59"/>
-      <c r="V38" s="61"/>
-      <c r="AN38" s="54"/>
-      <c r="AO38" s="54"/>
-      <c r="AP38" s="54"/>
-      <c r="AQ38" s="54"/>
-      <c r="AR38" s="54"/>
-      <c r="AS38" s="54"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="50"/>
+      <c r="U38" s="51"/>
+      <c r="V38" s="53"/>
+      <c r="AN38" s="46"/>
+      <c r="AO38" s="46"/>
+      <c r="AP38" s="46"/>
+      <c r="AQ38" s="46"/>
+      <c r="AR38" s="46"/>
+      <c r="AS38" s="46"/>
     </row>
     <row r="39" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="47" t="s">
         <v>9</v>
       </c>
       <c r="B39" s="22"/>
@@ -3217,29 +3766,29 @@
       <c r="F39" s="26"/>
       <c r="G39" s="26"/>
       <c r="H39" s="26"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="60"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="52"/>
       <c r="M39" s="34"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="61"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="53"/>
       <c r="R39" s="34"/>
-      <c r="S39" s="57"/>
-      <c r="T39" s="58"/>
-      <c r="U39" s="59"/>
-      <c r="V39" s="61"/>
-      <c r="AN39" s="54"/>
-      <c r="AO39" s="54"/>
-      <c r="AP39" s="54"/>
-      <c r="AQ39" s="54"/>
-      <c r="AR39" s="54"/>
-      <c r="AS39" s="54"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="50"/>
+      <c r="U39" s="51"/>
+      <c r="V39" s="53"/>
+      <c r="AN39" s="46"/>
+      <c r="AO39" s="46"/>
+      <c r="AP39" s="46"/>
+      <c r="AQ39" s="46"/>
+      <c r="AR39" s="46"/>
+      <c r="AS39" s="46"/>
     </row>
     <row r="40" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B40" s="22"/>
@@ -3249,29 +3798,29 @@
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
       <c r="H40" s="26"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="60"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="52"/>
       <c r="M40" s="34"/>
-      <c r="N40" s="57"/>
-      <c r="O40" s="58"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="61"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="53"/>
       <c r="R40" s="34"/>
-      <c r="S40" s="57"/>
-      <c r="T40" s="58"/>
-      <c r="U40" s="59"/>
-      <c r="V40" s="61"/>
-      <c r="AN40" s="54"/>
-      <c r="AO40" s="54"/>
-      <c r="AP40" s="54"/>
-      <c r="AQ40" s="54"/>
-      <c r="AR40" s="54"/>
-      <c r="AS40" s="54"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="50"/>
+      <c r="U40" s="51"/>
+      <c r="V40" s="53"/>
+      <c r="AN40" s="46"/>
+      <c r="AO40" s="46"/>
+      <c r="AP40" s="46"/>
+      <c r="AQ40" s="46"/>
+      <c r="AR40" s="46"/>
+      <c r="AS40" s="46"/>
     </row>
     <row r="41" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="47" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="22"/>
@@ -3281,29 +3830,29 @@
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="60"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="52"/>
       <c r="M41" s="34"/>
-      <c r="N41" s="57"/>
-      <c r="O41" s="58"/>
-      <c r="P41" s="59"/>
-      <c r="Q41" s="61"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="50"/>
+      <c r="P41" s="51"/>
+      <c r="Q41" s="53"/>
       <c r="R41" s="34"/>
-      <c r="S41" s="57"/>
-      <c r="T41" s="58"/>
-      <c r="U41" s="59"/>
-      <c r="V41" s="61"/>
-      <c r="AN41" s="54"/>
-      <c r="AO41" s="54"/>
-      <c r="AP41" s="54"/>
-      <c r="AQ41" s="54"/>
-      <c r="AR41" s="54"/>
-      <c r="AS41" s="54"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="50"/>
+      <c r="U41" s="51"/>
+      <c r="V41" s="53"/>
+      <c r="AN41" s="46"/>
+      <c r="AO41" s="46"/>
+      <c r="AP41" s="46"/>
+      <c r="AQ41" s="46"/>
+      <c r="AR41" s="46"/>
+      <c r="AS41" s="46"/>
     </row>
     <row r="42" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="47" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="22"/>
@@ -3313,29 +3862,29 @@
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
       <c r="H42" s="26"/>
-      <c r="I42" s="57"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="60"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="50"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="52"/>
       <c r="M42" s="34"/>
-      <c r="N42" s="57"/>
-      <c r="O42" s="58"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="61"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="50"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="53"/>
       <c r="R42" s="34"/>
-      <c r="S42" s="57"/>
-      <c r="T42" s="58"/>
-      <c r="U42" s="59"/>
-      <c r="V42" s="61"/>
-      <c r="AN42" s="54"/>
-      <c r="AO42" s="54"/>
-      <c r="AP42" s="54"/>
-      <c r="AQ42" s="54"/>
-      <c r="AR42" s="54"/>
-      <c r="AS42" s="54"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="50"/>
+      <c r="U42" s="51"/>
+      <c r="V42" s="53"/>
+      <c r="AN42" s="46"/>
+      <c r="AO42" s="46"/>
+      <c r="AP42" s="46"/>
+      <c r="AQ42" s="46"/>
+      <c r="AR42" s="46"/>
+      <c r="AS42" s="46"/>
     </row>
     <row r="43" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="47" t="s">
         <v>13</v>
       </c>
       <c r="B43" s="22"/>
@@ -3345,26 +3894,26 @@
       <c r="F43" s="26"/>
       <c r="G43" s="26"/>
       <c r="H43" s="26"/>
-      <c r="I43" s="57"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="59"/>
-      <c r="L43" s="60"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="52"/>
       <c r="M43" s="34"/>
-      <c r="N43" s="57"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="59"/>
-      <c r="Q43" s="61"/>
+      <c r="N43" s="49"/>
+      <c r="O43" s="50"/>
+      <c r="P43" s="51"/>
+      <c r="Q43" s="53"/>
       <c r="R43" s="34"/>
-      <c r="S43" s="57"/>
-      <c r="T43" s="58"/>
-      <c r="U43" s="59"/>
-      <c r="V43" s="61"/>
-      <c r="AN43" s="54"/>
-      <c r="AO43" s="54"/>
-      <c r="AP43" s="54"/>
-      <c r="AQ43" s="54"/>
-      <c r="AR43" s="54"/>
-      <c r="AS43" s="54"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="50"/>
+      <c r="U43" s="51"/>
+      <c r="V43" s="53"/>
+      <c r="AN43" s="46"/>
+      <c r="AO43" s="46"/>
+      <c r="AP43" s="46"/>
+      <c r="AQ43" s="46"/>
+      <c r="AR43" s="46"/>
+      <c r="AS43" s="46"/>
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
@@ -4201,134 +4750,259 @@
   </sheetData>
   <autoFilter ref="A5:AS2327" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="7">
+    <mergeCell ref="A1:H2"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="M4:Q4"/>
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="J619:J743 J745 J747 J749 J751 J753 J755 J757 J759 J761:J767 J915:J1038 J1040:J1177 J1182:J1196 J1201:J1205 J1210:J1259 J1263:J1287 J1289:J1381 J1385:J1409 J1411:J1470 J1472:J1558 J1597:J1618 J1755:J1756 J1759:J1786 J1914:J1955 J1958:J1960 J1963 J1965:J1967 J1970:J2007 J2010:J2050 J2053:J2075 J2078:J2081 J2084 J2086:J2088 J2091:J2132 J2328:J65040 J5:J6 O619:O743 O745 O747 O749 O751 O753 O755 O757 O759 O761:O767 O915:O1038 O1040:O1177 O1182:O1196 O1201:O1205 O1210:O1259 O1263:O1287 O1289:O1381 O1385:O1409 O1411:O1470 O1472:O1558 O1597:O1618 O1755:O1756 O1759:O1786 O1914:O1955 O1958:O1960 O1963 O1965:O1967 O1970:O2007 O2010:O2050 O2053:O2075 O2078:O2081 O2084 O2086:O2088 O2091:O2132 O2328:O65040 O5:O6 O8:O602 J8:J602">
-    <cfRule type="cellIs" dxfId="46" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="117" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="118" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="119" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I69 N8:N69">
-    <cfRule type="cellIs" dxfId="43" priority="60" operator="equal">
+  <conditionalFormatting sqref="N8:N69 I8:I15 I19:I69">
+    <cfRule type="cellIs" dxfId="99" priority="109" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="110" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="111" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="112" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="113" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I69 N8:N69">
-    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
+  <conditionalFormatting sqref="N8:N69 I8:I15 I19:I69">
+    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="95" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T619:T743 T745 T747 T749 T751 T753 T755 T757 T759 T761:T767 T915:T1038 T1040:T1177 T1182:T1196 T1201:T1205 T1210:T1259 T1263:T1287 T1289:T1381 T1385:T1409 T1411:T1470 T1472:T1558 T1597:T1618 T1755:T1756 T1759:T1786 T1914:T1955 T1958:T1960 T1963 T1965:T1967 T1970:T2007 T2010:T2050 T2053:T2075 T2078:T2081 T2084 T2086:T2088 T2091:T2132 T2328:T65040 T5:T6 T8:T602">
-    <cfRule type="cellIs" dxfId="36" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="84" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="85" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="86" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:S69">
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="79" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="80" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="81" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="82" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="83" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:S69">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="77" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="78" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="cellIs" dxfId="26" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="74" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="75" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="76" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="69" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="70" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="71" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="72" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="67" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="68" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S7">
-    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="64" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="65" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="66" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
+    <cfRule type="cellIs" dxfId="69" priority="59" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="60" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="61" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="62" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="63" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7">
+    <cfRule type="cellIs" dxfId="64" priority="57" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="58" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" dxfId="62" priority="52" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="53" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="54" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="55" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="56" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" dxfId="57" priority="50" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="51" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="55" priority="45" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="46" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="47" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="48" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="50" priority="43" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="26" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
     <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
@@ -4345,7 +5019,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R7">
+  <conditionalFormatting sqref="I17">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
@@ -4353,7 +5027,7 @@
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="I18">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
@@ -4370,7 +5044,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="I18">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
@@ -4380,10 +5054,10 @@
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P63:P64 K63:K64 U63:U64" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I69 S8:S69 N8:N69 M7 R7" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8:S69 N8:N69 M7 R7 I7:I69" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B12:B69 B7:B9" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B7:B9 B12:B69" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4401,7 +5075,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
     <col min="5" max="5" width="43.140625" customWidth="1"/>
@@ -4469,7 +5143,7 @@
       <c r="D4" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="40" t="s">
         <v>110</v>
       </c>
       <c r="F4" s="21" t="s">
@@ -4667,23 +5341,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -4809,10 +5466,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4834,19 +5518,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualización Documento salida TP N° 12
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Desktop\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joaquin2\Estudio\Ingenieria en Sistemas\4to Año\ISW - Ingeniería de Software\Repositorio\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFF05D1-287B-449D-8662-BCE8B5FA99DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B80373-6C44-402F-9154-E0051A60BAD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="185">
   <si>
     <t>TC_001</t>
   </si>
@@ -479,9 +479,6 @@
 El sistema muestra un mensaje de error "Debe seleccionar una forma de pago".</t>
   </si>
   <si>
-    <t>Pedir un producto específico(Con tarjeta ingresando mal el numero de tarjeta)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
 2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
 3. El solicitante no adjunta una foto de los auriculares.
@@ -503,9 +500,6 @@
 9. El sistema valida que la tarjeta de creditosea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "La tarjeta tiene que ser visa"</t>
   </si>
   <si>
-    <t>Pedir un producto específico(ingresando datos distintos del titular)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
 2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
 3. El solicitante no adjunta una foto de los auriculares.
@@ -550,6 +544,323 @@
 7. El solicitante selecciona la opcion "Siguiente"
 8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC 123
 9. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico (ingresando datos distintos del titular)</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico (Con tarjeta ingresando mal el numero de tarjeta)</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de credito sea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "los datos ingresados, no coinciden con los del titular de la tarjeta"</t>
+  </si>
+  <si>
+    <t>En el sistema el mes es 10 y el año 2019</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 09/2019 y CVC 123
+9. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de credito sea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "La tarjeta debe tener mes/año de vencimiento igual o posterior a 10/2019"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de credito sea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "La tarjeta tiene que ser visa"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de credito sea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "Date should not be before minimal date" y muestra ¿Cuando desea recibir el pedido? y  el detalle del pedido</t>
+  </si>
+  <si>
+    <t>1.Ingresar al sistema para Pedir "lo que sea".
+2. Ingresar una descripción del Producto "Auriculares Bluethoot Philips"
+3. Adjuntar una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. Seleccionar la direccion del comercio de desde el mapa de Google Maps
+5. Seleccionar la opcion "Siguiente"
+6. Ingresar la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: ddd, y seleccionar la ciudad Ciudad: Capital
+7. Seleccionar la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>El sistema permite el ingreso de una tarjeta con fecha de vencimiento anterior a la fecha actual</t>
+  </si>
+  <si>
+    <t>29b</t>
+  </si>
+  <si>
+    <t>Ingreso de tarjeta vencida</t>
+  </si>
+  <si>
+    <t>Ingreso de tarjeta con formato mes/año distinto a MM/AAAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+8. El sistema solo deja ingresar caracteres numéricos al campo fecha de vencimiento.
+</t>
+  </si>
+  <si>
+    <t>Ingreso de tarjeta con CVC no numérico</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de credito sea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "La tarjeta debe tener un CVC númerico"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de credito sea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "el cvc tiene formato incorrecto"</t>
+  </si>
+  <si>
+    <t>30b</t>
+  </si>
+  <si>
+    <t>Ingreso de tarjeta con CVC con menos de 3 dígitos</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de credito sea Visa y tenga un formato correcto, y no lo es. El sistema muestra un mensaje de error "La tarjeta debe tener un CVC de 3 dígitos"</t>
+  </si>
+  <si>
+    <t>30c</t>
+  </si>
+  <si>
+    <t>Ingreso de tarjeta con CVC con más de 3 dígitos</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC 4444
+9. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC 44
+9. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC aaa
+9. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento QQ/QWER y CVC 123
+</t>
+  </si>
+  <si>
+    <t>Ingeso sin seleccionar forma de entrega</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC 444
+9. El solicitante selecciona la opcion "Siguiente"
+10. El solicitante NO selecciona forma de entrega. 
+11. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de creditosea Visa y tenga un formato correcto, muestra ¿Cuando desea recibir el pedido? y  el detalle del pedido
+11. El sistema muestra un mensaje de error "Debe seleccionar una forma de entrega".</t>
+  </si>
+  <si>
+    <t>Ingreso con hora/fecha anterior a la actual</t>
+  </si>
+  <si>
+    <t>En el sistema el día es 17, el mes es 10, el año 2019 y la hora 20:00</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de creditosea Visa y tenga un formato correcto, muestra ¿Cuando desea recibir el pedido? y  el detalle del pedido
+11. El sistema muestra el mensaje "Debe indicar una fecha/hora posterior a la actual".</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
+9. El sistema valida que la tarjeta de creditosea Visa y tenga un formato correcto, muestra ¿Cuando desea recibir el pedido? y  el detalle del pedido
+11. El sistema muestra el mensaje "Felicitaciones, su pedido sera entregado el dia 17/10/2019 a las 19:30 Hs." y registra el nuevo pedido.</t>
+  </si>
+  <si>
+    <t>El sistema permite el ingreso de una fecha/hora anterior a la actual</t>
+  </si>
+  <si>
+    <t>Menor</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(sin descripcion ni direccion de comercio)</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(foto con formato distinto de JPG)</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(sin direccion de entrega)</t>
+  </si>
+  <si>
+    <t>Pedir un producto específico(con letras en el campo Nro. De la direccion de entrega)</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante no ingresa una descripción del Producto
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante no ingresa la direccion del comercio en forma textual y no ingresa un punto del mapa desde Google Maps
+5. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y el sistema muestra mensaje de error "No ingreso una descripcion del producto" y "No ingreso una direccion valida ni selecciono una ubicacion en el mapa"</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato PNG y con un tamaño de 5 Mbytes
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:567, Ciudad: Cordoba
+5. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio ingresada este completa y en formato valido y muestra mensaje de error "El formato de la foto adjuntada no es JPG" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante selecciona la direccion del comercio de desde el mapa de Google Maps
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante no ingresa la direccion de entrega
+7. El solicitante selecciona la opcion "Siguiente"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio se selecciono desde Google Maps y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra un mensaje de error "No ingreso una direccion de entrega".
+</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante adjunta una foto de los auriculares en formato JPG y con un tamaño de 5 Mbytes
+4. El solicitante selecciona la direccion del comercio de desde el mapa de Google Maps
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: ddd, y selecciona la ciudad Ciudad: Capital
+7. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>1. El sistema muestra la pantalla para realizar pedido de "lo que sea".
+5. El sistema valida que se ingreso una descripcion alfanumerica, que la foto ingresada sea de formato JPG y no supere los 5 MBytes, que la direccion del comercio se selecciono desde Google Maps y muestra la pantalla de Detalle de Entrega.
+7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra mensaje de error "Numero de direccion de entrega debe ser numerico"</t>
+  </si>
+  <si>
+    <t>El sistema permite el ingreso de fotos de formato distinto de JPG</t>
+  </si>
+  <si>
+    <t>1. Ingresar al sistema para Pedir "lo que sea".
+2. Ingresar una descripción del Producto "Auriculares Bluethoot Philips"
+3. Adjuntar una foto de los auriculares en formato PNG y con un tamaño de 5 MBytes
+4. Ingresar la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:567, Ciudad: Cordoba
+5. Releccionar la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t>El sistema permite el ingreso de letras en el campo Nro de la direccion de entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar al sistema para Pedir "lo que sea". 
+2. Ingresar una descripción del Producto "Auriculares Bluethoot Philips"
+3. No adjuntar foto
+4. 4. Ingresar la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:567, Ciudad: Cordoba
+5. Seleccionar la opcion "Siguiente"
+6. Ingresar la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: Nro.:450,, y seleccionar la ciudad Ciudad: Capital
+7. Seleccionar la opcion "Siguiente"
+8. Seleccionar forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 09/2019 y CVC 123
+9. Seleccionar la opcion "Siguiente"
+</t>
+  </si>
+  <si>
+    <t>1. El Solicitante ingresa al sistema para Pedir "lo que sea".
+2. El Solicitante ingresa una descripción del Producto "Auriculares Bluethoot Philips"
+3. El solicitante no adjunta una foto de los auriculares.
+4. El solicitante ingresa la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:450, Ciudad: Cordoba y una referencia "Famacity".
+5. El solicitante selecciona la opcion "Siguiente"
+6. El solicitante ingresa la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: 85,  selecciona la ciudad Ciudad: Capital y una referencia "Casa rosa"
+7. El solicitante selecciona la opcion "Siguiente"
+8. El solicitante selecciona forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 10/2019 y CVC 444
+9. El solicitante selecciona la opcion "Siguiente"
+10. El solicitante selecciona que desea recibir el producto en la fecha 17/10/2019 y hora 19:30 
+11. El solicitante selecciona la opcion "Siguiente"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar al sistema para Pedir "lo que sea". 
+2. Ingresar una descripción del Producto "Auriculares Bluethoot Philips"
+3. No adjuntar foto
+4. 4. Ingresar la direccion del comercio de la siguiente manera, Calle: Gral. Paz, Nro.:567, Ciudad: Cordoba
+5. Seleccionar la opcion "Siguiente"
+6. Ingresar la direccion de entrega de la siguiente manera, Calle: Chacabuco, Nro.: Nro.:450,, y seleccionar la ciudad Ciudad: Capital
+7. Seleccionar la opcion "Siguiente"
+8. Seleccionar forma de pago tarjeta Visa Nro de tarjeta 4444 3333 2222 1111, Titular de la tarjeta Juan Perez, fecha de vencimiento 09/2019 y CVC 123
+9. Seleccionar la opcion "Siguiente"
+10. Seleccionar que se desea recibir el producto en la fecha 17/10/2019 y hora 19:30 
+11. Seleccionar la opcion "Siguiente"
+</t>
   </si>
 </sst>
 </file>
@@ -955,7 +1266,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1124,6 +1435,53 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1138,7 +1496,129 @@
     <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="99">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="51"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2161,11 +2641,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS69"/>
+  <dimension ref="A1:AS72"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2655,22 +3135,39 @@
       <c r="AR10" s="46"/>
       <c r="AS10" s="46"/>
     </row>
-    <row r="11" spans="1:45" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+    <row r="11" spans="1:45" s="11" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="49"/>
+      <c r="D11" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="G11" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="I11" s="65" t="s">
+        <v>98</v>
+      </c>
       <c r="J11" s="50"/>
       <c r="K11" s="51"/>
-      <c r="L11" s="52"/>
+      <c r="L11" s="76">
+        <v>43755</v>
+      </c>
       <c r="M11" s="34"/>
       <c r="N11" s="49"/>
       <c r="O11" s="50"/>
@@ -2688,23 +3185,41 @@
       <c r="AR11" s="46"/>
       <c r="AS11" s="46"/>
     </row>
-    <row r="12" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+    <row r="12" spans="1:45" s="11" customFormat="1" ht="132" x14ac:dyDescent="0.2">
+      <c r="A12" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22">
+      <c r="B12" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="69">
         <v>6</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="52"/>
+      <c r="D12" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="72" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="75" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="64"/>
+      <c r="K12" s="62">
+        <v>2</v>
+      </c>
+      <c r="L12" s="63">
+        <v>43755</v>
+      </c>
       <c r="M12" s="34"/>
       <c r="N12" s="49"/>
       <c r="O12" s="50"/>
@@ -2722,23 +3237,39 @@
       <c r="AR12" s="46"/>
       <c r="AS12" s="46"/>
     </row>
-    <row r="13" spans="1:45" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
+    <row r="13" spans="1:45" s="11" customFormat="1" ht="192" x14ac:dyDescent="0.2">
+      <c r="A13" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="52"/>
+      <c r="D13" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="I13" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="64"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="63">
+        <v>43755</v>
+      </c>
       <c r="M13" s="34"/>
       <c r="N13" s="49"/>
       <c r="O13" s="50"/>
@@ -2756,23 +3287,41 @@
       <c r="AR13" s="46"/>
       <c r="AS13" s="46"/>
     </row>
-    <row r="14" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
+    <row r="14" spans="1:45" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.2">
+      <c r="A14" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22">
+      <c r="B14" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="69">
         <v>22</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="52"/>
+      <c r="D14" s="69" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="G14" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="75" t="s">
+        <v>106</v>
+      </c>
+      <c r="I14" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" s="64"/>
+      <c r="K14" s="62">
+        <v>3</v>
+      </c>
+      <c r="L14" s="63">
+        <v>43755</v>
+      </c>
       <c r="M14" s="34"/>
       <c r="N14" s="49"/>
       <c r="O14" s="50"/>
@@ -2795,7 +3344,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C15" s="22">
         <v>25</v>
@@ -2844,7 +3393,9 @@
       <c r="A16" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="22" t="s">
+        <v>133</v>
+      </c>
       <c r="C16" s="22">
         <v>26</v>
       </c>
@@ -2893,25 +3444,25 @@
         <v>49</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C17" s="21">
         <v>27</v>
       </c>
       <c r="D17" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="G17" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="F17" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="G17" s="40" t="s">
-        <v>125</v>
-      </c>
       <c r="H17" s="40" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>98</v>
@@ -2949,19 +3500,19 @@
         <v>28</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="H18" s="40" t="s">
-        <v>128</v>
       </c>
       <c r="I18" s="15" t="s">
         <v>107</v>
@@ -2988,23 +3539,39 @@
       <c r="AR18" s="46"/>
       <c r="AS18" s="46"/>
     </row>
-    <row r="19" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" s="11" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A19" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="C19" s="22">
         <v>29</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="49"/>
+      <c r="D19" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>107</v>
+      </c>
       <c r="J19" s="50"/>
       <c r="K19" s="51"/>
-      <c r="L19" s="52"/>
+      <c r="L19" s="76">
+        <v>43755</v>
+      </c>
       <c r="M19" s="34"/>
       <c r="N19" s="49"/>
       <c r="O19" s="50"/>
@@ -3022,23 +3589,37 @@
       <c r="AR19" s="46"/>
       <c r="AS19" s="46"/>
     </row>
-    <row r="20" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" s="11" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A20" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22">
-        <v>30</v>
-      </c>
-      <c r="D20" s="22"/>
+      <c r="B20" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="69" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>144</v>
+      </c>
       <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="49"/>
+      <c r="F20" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G20" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="I20" s="66" t="s">
+        <v>98</v>
+      </c>
       <c r="J20" s="50"/>
       <c r="K20" s="51"/>
-      <c r="L20" s="52"/>
+      <c r="L20" s="52">
+        <v>43755</v>
+      </c>
       <c r="M20" s="34"/>
       <c r="N20" s="49"/>
       <c r="O20" s="50"/>
@@ -3056,23 +3637,39 @@
       <c r="AR20" s="46"/>
       <c r="AS20" s="46"/>
     </row>
-    <row r="21" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" s="11" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A21" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="22" t="s">
+        <v>133</v>
+      </c>
       <c r="C21" s="22">
-        <v>33</v>
-      </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="49"/>
+        <v>30</v>
+      </c>
+      <c r="D21" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>98</v>
+      </c>
       <c r="J21" s="50"/>
       <c r="K21" s="51"/>
-      <c r="L21" s="52"/>
+      <c r="L21" s="52">
+        <v>43755</v>
+      </c>
       <c r="M21" s="34"/>
       <c r="N21" s="49"/>
       <c r="O21" s="50"/>
@@ -3090,23 +3687,39 @@
       <c r="AR21" s="46"/>
       <c r="AS21" s="46"/>
     </row>
-    <row r="22" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" s="11" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A22" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22">
-        <v>34</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="49"/>
+      <c r="B22" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="69" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" s="49" t="s">
+        <v>98</v>
+      </c>
       <c r="J22" s="50"/>
       <c r="K22" s="51"/>
-      <c r="L22" s="52"/>
+      <c r="L22" s="76">
+        <v>43755</v>
+      </c>
       <c r="M22" s="34"/>
       <c r="N22" s="49"/>
       <c r="O22" s="50"/>
@@ -3124,21 +3737,39 @@
       <c r="AR22" s="46"/>
       <c r="AS22" s="46"/>
     </row>
-    <row r="23" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" s="11" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A23" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="49"/>
+      <c r="B23" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="H23" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="49" t="s">
+        <v>98</v>
+      </c>
       <c r="J23" s="50"/>
       <c r="K23" s="51"/>
-      <c r="L23" s="52"/>
+      <c r="L23" s="76">
+        <v>43755</v>
+      </c>
       <c r="M23" s="34"/>
       <c r="N23" s="49"/>
       <c r="O23" s="50"/>
@@ -3156,21 +3787,39 @@
       <c r="AR23" s="46"/>
       <c r="AS23" s="46"/>
     </row>
-    <row r="24" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" s="11" customFormat="1" ht="288" x14ac:dyDescent="0.2">
       <c r="A24" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="49"/>
+      <c r="B24" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="22">
+        <v>33</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="G24" s="72" t="s">
+        <v>160</v>
+      </c>
+      <c r="H24" s="72" t="s">
+        <v>160</v>
+      </c>
+      <c r="I24" s="49" t="s">
+        <v>98</v>
+      </c>
       <c r="J24" s="50"/>
       <c r="K24" s="51"/>
-      <c r="L24" s="52"/>
+      <c r="L24" s="52">
+        <v>43755</v>
+      </c>
       <c r="M24" s="34"/>
       <c r="N24" s="49"/>
       <c r="O24" s="50"/>
@@ -3188,21 +3837,41 @@
       <c r="AR24" s="46"/>
       <c r="AS24" s="46"/>
     </row>
-    <row r="25" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" s="11" customFormat="1" ht="288" x14ac:dyDescent="0.2">
       <c r="A25" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="49"/>
+      <c r="B25" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="22">
+        <v>34</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="70" t="s">
+        <v>183</v>
+      </c>
+      <c r="G25" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="I25" s="49" t="s">
+        <v>107</v>
+      </c>
       <c r="J25" s="50"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="52"/>
+      <c r="K25" s="51">
+        <v>10</v>
+      </c>
+      <c r="L25" s="52">
+        <v>43755</v>
+      </c>
       <c r="M25" s="34"/>
       <c r="N25" s="49"/>
       <c r="O25" s="50"/>
@@ -3228,7 +3897,7 @@
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
+      <c r="F26" s="70"/>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
       <c r="I26" s="49"/>
@@ -3260,7 +3929,7 @@
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
+      <c r="F27" s="70"/>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
       <c r="I27" s="49"/>
@@ -3289,10 +3958,10 @@
         <v>60</v>
       </c>
       <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="40"/>
       <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
+      <c r="F28" s="72"/>
       <c r="G28" s="40"/>
       <c r="H28" s="26"/>
       <c r="I28" s="49"/>
@@ -3321,10 +3990,10 @@
         <v>61</v>
       </c>
       <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="40"/>
       <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
+      <c r="F29" s="72"/>
       <c r="G29" s="40"/>
       <c r="H29" s="26"/>
       <c r="I29" s="49"/>
@@ -3356,7 +4025,7 @@
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="26"/>
-      <c r="F30" s="40"/>
+      <c r="F30" s="72"/>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
       <c r="I30" s="49"/>
@@ -3385,10 +4054,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
+      <c r="C31" s="40"/>
       <c r="D31" s="22"/>
       <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
       <c r="I31" s="49"/>
@@ -3417,10 +4086,10 @@
         <v>2</v>
       </c>
       <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
+      <c r="C32" s="40"/>
       <c r="D32" s="22"/>
       <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="F32" s="70"/>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
       <c r="I32" s="49"/>
@@ -3801,7 +4470,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
+      <c r="C44" s="22"/>
       <c r="D44" s="21"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
@@ -3833,7 +4502,7 @@
         <v>15</v>
       </c>
       <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
+      <c r="C45" s="22"/>
       <c r="D45" s="21"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
@@ -3865,7 +4534,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="21"/>
       <c r="E46" s="26"/>
       <c r="F46" s="26"/>
@@ -4601,7 +5270,7 @@
         <v>39</v>
       </c>
       <c r="B69" s="21"/>
-      <c r="C69" s="27"/>
+      <c r="C69" s="21"/>
       <c r="D69" s="27"/>
       <c r="E69" s="22"/>
       <c r="F69" s="26"/>
@@ -4628,6 +5297,15 @@
       <c r="AR69" s="7"/>
       <c r="AS69" s="7"/>
     </row>
+    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="C70" s="21"/>
+    </row>
+    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="C71" s="21"/>
+    </row>
+    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="C72" s="27"/>
+    </row>
   </sheetData>
   <autoFilter ref="A5:AS2327" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="7">
@@ -4639,90 +5317,151 @@
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="D3:F3"/>
   </mergeCells>
-  <conditionalFormatting sqref="J619:J743 J745 J747 J749 J751 J753 J755 J757 J759 J761:J767 J915:J1038 J1040:J1177 J1182:J1196 J1201:J1205 J1210:J1259 J1263:J1287 J1289:J1381 J1385:J1409 J1411:J1470 J1472:J1558 J1597:J1618 J1755:J1756 J1759:J1786 J1914:J1955 J1958:J1960 J1963 J1965:J1967 J1970:J2007 J2010:J2050 J2053:J2075 J2078:J2081 J2084 J2086:J2088 J2091:J2132 J2328:J65040 J5:J6 O619:O743 O745 O747 O749 O751 O753 O755 O757 O759 O761:O767 O915:O1038 O1040:O1177 O1182:O1196 O1201:O1205 O1210:O1259 O1263:O1287 O1289:O1381 O1385:O1409 O1411:O1470 O1472:O1558 O1597:O1618 O1755:O1756 O1759:O1786 O1914:O1955 O1958:O1960 O1963 O1965:O1967 O1970:O2007 O2010:O2050 O2053:O2075 O2078:O2081 O2084 O2086:O2088 O2091:O2132 O2328:O65040 O5:O6 O8:O602 J8:J602">
-    <cfRule type="cellIs" dxfId="81" priority="117" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="J619:J743 J745 J747 J749 J751 J753 J755 J757 J759 J761:J767 J915:J1038 J1040:J1177 J1182:J1196 J1201:J1205 J1210:J1259 J1263:J1287 J1289:J1381 J1385:J1409 J1411:J1470 J1472:J1558 J1597:J1618 J1755:J1756 J1759:J1786 J1914:J1955 J1958:J1960 J1963 J1965:J1967 J1970:J2007 J2010:J2050 J2053:J2075 J2078:J2081 J2084 J2086:J2088 J2091:J2132 J2328:J65040 J5:J6 O619:O743 O745 O747 O749 O751 O753 O755 O757 O759 O761:O767 O915:O1038 O1040:O1177 O1182:O1196 O1201:O1205 O1210:O1259 O1263:O1287 O1289:O1381 O1385:O1409 O1411:O1470 O1472:O1558 O1597:O1618 O1755:O1756 O1759:O1786 O1914:O1955 O1958:O1960 O1963 O1965:O1967 O1970:O2007 O2010:O2050 O2053:O2075 O2078:O2081 O2084 O2086:O2088 O2091:O2132 O2328:O65040 O5:O6 O8:O602 J8:J11 J15:J602">
+    <cfRule type="cellIs" dxfId="98" priority="134" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="118" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="135" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="119" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="136" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:N69 I8:I15 I19:I69">
-    <cfRule type="cellIs" dxfId="78" priority="109" operator="equal">
+  <conditionalFormatting sqref="N8:N69 I8:I10 I19:I69 I15">
+    <cfRule type="cellIs" dxfId="95" priority="126" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="127" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="128" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="129" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="130" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:N69 I8:I15 I19:I69">
-    <cfRule type="cellIs" dxfId="73" priority="94" operator="equal">
+  <conditionalFormatting sqref="N8:N69 I8:I10 I19:I69 I15">
+    <cfRule type="cellIs" dxfId="90" priority="111" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="112" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T619:T743 T745 T747 T749 T751 T753 T755 T757 T759 T761:T767 T915:T1038 T1040:T1177 T1182:T1196 T1201:T1205 T1210:T1259 T1263:T1287 T1289:T1381 T1385:T1409 T1411:T1470 T1472:T1558 T1597:T1618 T1755:T1756 T1759:T1786 T1914:T1955 T1958:T1960 T1963 T1965:T1967 T1970:T2007 T2010:T2050 T2053:T2075 T2078:T2081 T2084 T2086:T2088 T2091:T2132 T2328:T65040 T5:T6 T8:T602">
-    <cfRule type="cellIs" dxfId="71" priority="84" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="101" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="85" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="102" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="86" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="103" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:S69">
-    <cfRule type="cellIs" dxfId="68" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="96" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="97" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="98" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="99" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="100" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:S69">
-    <cfRule type="cellIs" dxfId="63" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="94" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="95" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="cellIs" dxfId="61" priority="74" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="91" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="75" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="92" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="93" stopIfTrue="1" operator="equal">
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
+    <cfRule type="cellIs" dxfId="75" priority="86" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="87" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="88" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="89" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="90" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7">
+    <cfRule type="cellIs" dxfId="70" priority="84" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="85" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S7">
+    <cfRule type="cellIs" dxfId="68" priority="81" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="82" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="83" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7">
+    <cfRule type="cellIs" dxfId="65" priority="76" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="77" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="78" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="79" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="80" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7">
+    <cfRule type="cellIs" dxfId="60" priority="74" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="75" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
     <cfRule type="cellIs" dxfId="58" priority="69" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
@@ -4739,7 +5478,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7">
+  <conditionalFormatting sqref="I7">
     <cfRule type="cellIs" dxfId="53" priority="67" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
@@ -4747,168 +5486,168 @@
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S7">
-    <cfRule type="cellIs" dxfId="51" priority="64" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="51" priority="62" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="63" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="64" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="65" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="66" operator="equal">
       <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="65" stopIfTrue="1" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="66" stopIfTrue="1" operator="equal">
-      <formula>"Can't Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="48" priority="59" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="60" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="61" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="62" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="63" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="58" operator="equal">
-      <formula>"Fallo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="53" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="54" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="55" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="56" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
-      <formula>"Paso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="51" operator="equal">
-      <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="34" priority="45" operator="equal">
-      <formula>"To Be Completed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="46" operator="equal">
-      <formula>"Not Apply"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="47" operator="equal">
-      <formula>"Can't run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="48" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="49" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="29" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="60" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="61" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="27" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="45" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Not Apply"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"Can't run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="24" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+      <formula>"To Be Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+      <formula>"Not Apply"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+      <formula>"Can't run"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"Paso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Fallo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12:J14">
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Can't Run"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:I14">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"To Be Completed"</formula>
     </cfRule>
@@ -4925,7 +5664,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="I12:I14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Paso"</formula>
     </cfRule>
@@ -4952,8 +5691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F14" sqref="F11:F14"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5012,54 +5751,82 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A4" s="20">
+      <c r="A4" s="67">
         <v>1</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="71">
         <v>43755</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="68" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+    <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A5" s="67">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="B5" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="71">
+        <v>43755</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A6" s="67">
         <v>3</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="B6" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="71">
+        <v>43755</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="68" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
@@ -5108,10 +5875,10 @@
         <v>43755</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>111</v>
@@ -5134,10 +5901,10 @@
         <v>43755</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>111</v>
@@ -5149,29 +5916,57 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>9</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="39">
+        <v>43755</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>10</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="B13" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="71">
+        <v>43755</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="68" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
@@ -5250,23 +6045,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5392,10 +6170,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5417,19 +6222,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualización documento de salida TP N° 12
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joaquin2\Estudio\Ingenieria en Sistemas\4to Año\ISW - Ingeniería de Software\Repositorio\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECC4B7F-FBD1-4FA2-AA85-698285107F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F2A1CF-919C-403F-9013-D2B27441D733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1056,7 +1056,7 @@
 5. El sistema valida que se ingreso una descripcion alfanumerica,  que la direccion del comercio ingresada este completa y en formato valido y muestra la pantalla de Detalle de Entrega.
 7. El sistema valida que la direccion de entrega ingresada este completa y en formato valido y muestra la pantalla Detalle de Pago.
 9. El sistema valida que la tarjeta de creditosea Visa y tenga un formato correcto, muestra ¿Cuando desea recibir el pedido? y  el detalle del pedido
-11. El sistema muestramensajes de error "campo obligatorio" para fecha y para hora</t>
+11. El sistema muestra mensajes de error "campo obligatorio" para fecha y para hora</t>
   </si>
 </sst>
 </file>
@@ -2940,9 +2940,9 @@
   </sheetPr>
   <dimension ref="A1:AS72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6489,6 +6489,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -6614,24 +6631,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6647,28 +6671,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
se borra la linea 8 de bug, que estaba vacia
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 12/Documento_Salida_Casos_De_Prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joaquin2\Estudio\Ingenieria en Sistemas\4to Año\ISW - Ingeniería de Software\Repositorio\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmanuel\Desktop\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2044DEE3-ADDB-4AFB-BEF7-B0554557EE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783F8D9E-3F3F-4AAB-A821-EF6F60B6892C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -2943,9 +2943,9 @@
   </sheetPr>
   <dimension ref="A1:AS72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6108,10 +6108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6351,33 +6351,47 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>8</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="B11" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="39">
+        <v>43755</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>9</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="39">
+        <v>57</v>
+      </c>
+      <c r="C12" s="62">
         <v>43755</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" s="63" t="s">
-        <v>137</v>
+        <v>125</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>138</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>126</v>
@@ -6389,31 +6403,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>10</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="62">
-        <v>43755</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="H13" s="59" t="s">
-        <v>108</v>
-      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
@@ -6463,27 +6463,15 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="20">
-        <v>15</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F17" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Bloqueante,Critico,Severo,Menor,Cosmetico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18" xr:uid="{C5E3F37E-FB36-4F7F-99E9-6282EDC122A6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H17" xr:uid="{C5E3F37E-FB36-4F7F-99E9-6282EDC122A6}">
       <formula1>"Creado,En Desarrollo,En Prueba,Resuelto,Bloqueado,Cancelado,Cerrado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6492,6 +6480,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -6617,24 +6622,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6650,28 +6662,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>